<commit_message>
:sparkles: feat: enhance preprocessing with NER and improved validation, add comparison test
</commit_message>
<xml_diff>
--- a/data/processed/Hackathon Participa DF Data Processado.xlsx
+++ b/data/processed/Hackathon Participa DF Data Processado.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O99"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>1</v>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -811,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>1</v>
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
         <v>2</v>
@@ -1022,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L12" t="n">
         <v>6</v>
@@ -1105,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
         <v>1</v>
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
         <v>0</v>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -1365,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
         <v>0</v>
@@ -1377,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="O19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1561,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L23" t="n">
         <v>9</v>
@@ -1650,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
         <v>1</v>
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
         <v>4</v>
@@ -1671,7 +1671,7 @@
         <v>11</v>
       </c>
       <c r="O25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
         <v>1</v>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L27" t="n">
         <v>6</v>
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>1</v>
@@ -1987,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
         <v>1</v>
@@ -2036,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
         <v>1</v>
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" t="n">
         <v>1</v>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
         <v>1</v>
@@ -2296,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="K38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L38" t="n">
         <v>4</v>
@@ -2379,7 +2379,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
         <v>1</v>
@@ -2428,13 +2428,13 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
         <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
         <v>1</v>
@@ -2443,7 +2443,7 @@
         <v>1</v>
       </c>
       <c r="K41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" t="n">
         <v>7</v>
@@ -2581,7 +2581,7 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
@@ -2590,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" t="n">
         <v>1</v>
@@ -2602,7 +2602,7 @@
         <v>3</v>
       </c>
       <c r="O44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -2639,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="K45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L45" t="n">
         <v>0</v>
@@ -2826,7 +2826,7 @@
         <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
@@ -2835,7 +2835,7 @@
         <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L49" t="n">
         <v>0</v>
@@ -2847,7 +2847,7 @@
         <v>5</v>
       </c>
       <c r="O49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2933,7 +2933,7 @@
         <v>1</v>
       </c>
       <c r="K51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L51" t="n">
         <v>3</v>
@@ -3031,7 +3031,7 @@
         <v>1</v>
       </c>
       <c r="K53" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L53" t="n">
         <v>9</v>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
@@ -3080,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="K54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54" t="n">
         <v>0</v>
@@ -3092,7 +3092,7 @@
         <v>1</v>
       </c>
       <c r="O54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -3129,7 +3129,7 @@
         <v>1</v>
       </c>
       <c r="K55" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L55" t="n">
         <v>0</v>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56" t="n">
         <v>1</v>
@@ -3218,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
         <v>1</v>
@@ -3227,7 +3227,7 @@
         <v>1</v>
       </c>
       <c r="K57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L57" t="n">
         <v>4</v>
@@ -3239,7 +3239,7 @@
         <v>10</v>
       </c>
       <c r="O57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -3408,7 +3408,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" t="n">
         <v>1</v>
@@ -3702,13 +3702,13 @@
         <v>0</v>
       </c>
       <c r="F67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67" t="n">
         <v>1</v>
       </c>
       <c r="H67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="n">
         <v>1</v>
@@ -3717,7 +3717,7 @@
         <v>0</v>
       </c>
       <c r="K67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L67" t="n">
         <v>1</v>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68" t="n">
         <v>1</v>
@@ -3849,7 +3849,7 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" t="n">
         <v>1</v>
@@ -3864,7 +3864,7 @@
         <v>1</v>
       </c>
       <c r="K70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L70" t="n">
         <v>2</v>
@@ -3904,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="H71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" t="n">
         <v>0</v>
@@ -3913,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L71" t="n">
         <v>0</v>
@@ -3925,7 +3925,7 @@
         <v>1</v>
       </c>
       <c r="O71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -3947,7 +3947,7 @@
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" t="n">
         <v>1</v>
@@ -3996,7 +3996,7 @@
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
         <v>1</v>
@@ -4045,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" t="n">
         <v>1</v>
@@ -4149,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="H76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" t="n">
         <v>1</v>
@@ -4158,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="K76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L76" t="n">
         <v>4</v>
@@ -4170,7 +4170,7 @@
         <v>7</v>
       </c>
       <c r="O76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -4192,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77" t="n">
         <v>1</v>
@@ -4550,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="K84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L84" t="n">
         <v>1</v>
@@ -4590,7 +4590,7 @@
         <v>0</v>
       </c>
       <c r="H85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85" t="n">
         <v>1</v>
@@ -4599,7 +4599,7 @@
         <v>0</v>
       </c>
       <c r="K85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L85" t="n">
         <v>1</v>
@@ -4682,7 +4682,7 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87" t="n">
         <v>1</v>
@@ -4780,7 +4780,7 @@
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" t="n">
         <v>1</v>
@@ -4959,11 +4959,11 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Segundo o item 15.4.1 do Edital Concurso Público Nº 02/2026 - ACI, o candidato matriculado no curso de formação profissional percebe, a título de ajuda financeira, 50% (cinquenta por cento) do vencimento básico fixado para o padrão inicial do cargo, até a data de desligamento do curso de formação profissional, com base nesse item, solicito esclarecimentos da CGDF-DF se existe alguma ilegalidade ou impedimento para recebimento da ajuda financeira por candidatos que sejam servidores efetivos de outros entes federativos (União, Estados ou Municípios), que estejam em gozo de férias ou licença não remunerada para participar do curso de formação profissional do referido certame. Além disso, havendo impedimento legal, solicito orientação da CGDF-DF sobre como proceder durante a matrícula no curso de formação, para dirimir as dúvidas dos candidatos que se encontram nessa situação. Numa solicitação anterior à SEEC - Protocolo LAI-258453/2026 (328647128), foi informado que: Assunto: Protocolo LAI-258453/2026 1. Trata-se do Despacho ? SEEC/GAB/OUV (687532419), referente ao Protocolo LAI-258453/2026 (328647128), por meio do qual o interessadonsolicita informações sobre matrícula no curso de formação para o servidor efetivo de outros entes federativos (União, Estados ou Municípios), especialmente acerca da ajuda financeira, disposto no Edital Concurso Público Nº 02/2026 - ACI. 2. Assim, entende-se, que a consulta em tela deve ser encaminhada à unidade de gestão de pessoas do órgão de lotação do requerente, para que, à luz da legislação vigente, seja avaliada a possibilidade ou não do recebimento do valor da ajuda financeira referente ao curso de formação. 3. Em face das considerações apresentadas, encaminho os autos a essa Unidade para conhecimento e providências pertinentes. Diante dessa resposta emitida pela SEEC, encaminho para a CGDF-DF novo pedido de informações a respeito do questionamento em tela, visto que o cargo para o qual concorro no certame (Auditor de Controle Interno) faz parte da estrutura desta secretaria. Atenciosamente,</t>
+          <t>Respeitosamente, solicitam-se as seguintes informações: Funções de Integridade 1. Houve instituição do Programa de Integridade no Órgão/Entidade? Se houve qual o normativo? (EX: Portaria xxx/xxx publicada no DODF xxx). 2. A alta administração participou de eventos internos de integridade? 3. Há previsão de capacitação e treinamentos periódicos? 4. Há diretrizes formais para o gerenciamento de riscos para a integridade aprovadas pela Alta Administração? 5. Desenvolveu campanha própria de conscientização sobre assuntos relacionados com a agenda de integridade pública? 6. Realiza capacitações e/ou treinamentos em temas que fortalecem a cultura de integridade da organização? 7. A organização possui unidade responsável pela gestão de riscos? Gestão de Integridade 1. As diretrizes para a integridade pública foram formalizadas e aprovadas pela alta administração? (EX: programa ou políticas) 2. As competências da Unidade responsável pelo Programa de Integridade foram formalmente atribuídas? 3. Possui plano de integridade formalizado? 4. O plano de integridade possui prazo de vigência? 5. A autoridade máxima aprovou o plano de integridade? 6. O plano de integridade prevê a periodicidade para sua revisão? 7. O plano de integridade contempla medidas baseadas em riscos? 8. O plano de integridade contempla medidas para estabelecimento ou aperfeiçoamento das funções de integridade? 9. O plano de integridade contempla medidas para a realização de capacitações em temas relacionados à integridade pública? 10. O plano de integridade contempla a forma e periodicidade de monitoramento de suas medidas? 11 –Quais são os indicadores utilizados para monitoramento? 12. A unidade responsável pelo controle interno monitora o plano de integridade? 13. Os resultados do monitoramento do plano de integridade são periodicamente reportados ao dirigente máximo? 14. Possui iniciativas para expansão do alcance de seu programa de Integridade para as políticas públicas implementadas e monitoradas pelo órgão/entidade? Bem como para fornecedores e outras instituições privadas com as quais mantenha relação? Gestão de Riscos: 1. Há unidade responsável pela gestão de riscos? 2. Há política de gestão de riscos? 3. A metodologia de gestão de riscos prevê a categoria integridade? 4. Houve mapeamento de riscos na elaboração do Plano de Integridade? Capacidades Estatais: 1. Há unidade formalmente responsável pelo programa de integridade? 2. Os servidores designados possuem dedicação exclusiva? 3. Haveria necessidade de um número mínimo de servidores com dedicação exclusiva para implementar e monitorar o sistema de integridade? 4. O estado ofertou condições para o desenvolvimento das atividades relacionadas à Integridade Pública como, por exemplo: capacitação de pessoal, infraestrutura, canal eficaz de comunicação com o(s) órgão(s) responsável(eis) pela coordenação dos programas de integridade? 5. Há indicadores para monitoramento do programa de integridade estabelecidos de forma uniforme para todo o Distrito Federal? 6. Quais as maiores limitações / desafios para a implementação do programa de Integridade? 7. Quais as maiores limitações / desafios para o monitoramento do programa de Integridade?</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -4979,10 +4979,10 @@
         <v>0</v>
       </c>
       <c r="G93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" t="n">
         <v>1</v>
@@ -4991,16 +4991,16 @@
         <v>1</v>
       </c>
       <c r="K93" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L93" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="M93" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N93" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O93" t="n">
         <v>1</v>
@@ -5008,11 +5008,11 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Qual foi o critério usado como marco temporal de prazo para suspensão dos prazos de validade dos concursos da SEMOBDF 2023 COM DATA DE HOMOLOGAÇÃO EM 12/10/2023 Edital n° 62 e SSPDF 2023 COM DATA DE HOMOLOGAÇÃO EM 20/11/2023 Editais n° 53 e 54. Gostaria de saber a partir de QUANDO/QUAL DATA foi suspenso o prazo em cada um dos concursos e editais.</t>
+          <t>Segundo o item 15.4.1 do Edital Concurso Público Nº 02/2026 - ACI, o candidato matriculado no curso de formação profissional percebe, a título de ajuda financeira, 50% (cinquenta por cento) do vencimento básico fixado para o padrão inicial do cargo, até a data de desligamento do curso de formação profissional, com base nesse item, solicito esclarecimentos da CGDF-DF se existe alguma ilegalidade ou impedimento para recebimento da ajuda financeira por candidatos que sejam servidores efetivos de outros entes federativos (União, Estados ou Municípios), que estejam em gozo de férias ou licença não remunerada para participar do curso de formação profissional do referido certame. Além disso, havendo impedimento legal, solicito orientação da CGDF-DF sobre como proceder durante a matrícula no curso de formação, para dirimir as dúvidas dos candidatos que se encontram nessa situação. Numa solicitação anterior à SEEC - Protocolo LAI-258453/2026 (328647128), foi informado que: Assunto: Protocolo LAI-258453/2026 1. Trata-se do Despacho ? SEEC/GAB/OUV (687532419), referente ao Protocolo LAI-258453/2026 (328647128), por meio do qual o interessadonsolicita informações sobre matrícula no curso de formação para o servidor efetivo de outros entes federativos (União, Estados ou Municípios), especialmente acerca da ajuda financeira, disposto no Edital Concurso Público Nº 02/2026 - ACI. 2. Assim, entende-se, que a consulta em tela deve ser encaminhada à unidade de gestão de pessoas do órgão de lotação do requerente, para que, à luz da legislação vigente, seja avaliada a possibilidade ou não do recebimento do valor da ajuda financeira referente ao curso de formação. 3. Em face das considerações apresentadas, encaminho os autos a essa Unidade para conhecimento e providências pertinentes. Diante dessa resposta emitida pela SEEC, encaminho para a CGDF-DF novo pedido de informações a respeito do questionamento em tela, visto que o cargo para o qual concorro no certame (Auditor de Controle Interno) faz parte da estrutura desta secretaria. Atenciosamente,</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -5028,7 +5028,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -5037,117 +5037,117 @@
         <v>1</v>
       </c>
       <c r="J94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K94" t="n">
         <v>0</v>
       </c>
       <c r="L94" t="n">
+        <v>11</v>
+      </c>
+      <c r="M94" t="n">
         <v>3</v>
       </c>
-      <c r="M94" t="n">
-        <v>0</v>
-      </c>
       <c r="N94" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="O94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Olá! Quero ter acesso ao processo administrativo: 00037-12687439/2024-02 Autuação: G000025483 ORGAO: DETRAN CONTATO PARA RETORNO: Email: psyahoo@mega.com 11 789654123</t>
+          <t>Qual foi o critério usado como marco temporal de prazo para suspensão dos prazos de validade dos concursos da SEMOBDF 2023 COM DATA DE HOMOLOGAÇÃO EM 12/10/2023 Edital n° 62 e SSPDF 2023 COM DATA DE HOMOLOGAÇÃO EM 20/11/2023 Editais n° 53 e 54. Gostaria de saber a partir de QUANDO/QUAL DATA foi suspenso o prazo em cada um dos concursos e editais.</t>
         </is>
       </c>
       <c r="C95" t="n">
         <v>0</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95" t="n">
         <v>0</v>
       </c>
       <c r="I95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K95" t="n">
         <v>0</v>
       </c>
       <c r="L95" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N95" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Aconteceu um problema no meu computador e desde então não consigo encontrar e baixar o soft COMERCIOPLUS 2020. Estou com um enorme problema, pois durante todos esses anos os meus controles da minha propriedade comercial estão vinculados ao COMERCIOPLUS 2020. No momento estou sem acesso a todos os meus controles. Venho pedir encarecidamente a ajuda da DF Legal. Confiante na solução desse meu problema já agradeço atenção! OBS; Sou usuário do COMERCIOPLUS desde a versão 2012</t>
+          <t>Olá! Quero ter acesso ao processo administrativo: 00037-12687439/2024-02 Autuação: G000025483 ORGAO: DETRAN CONTATO PARA RETORNO: Email: psyahoo@mega.com 11 789654123</t>
         </is>
       </c>
       <c r="C96" t="n">
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J96" t="n">
         <v>1</v>
       </c>
       <c r="K96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M96" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N96" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O96" t="n">
         <v>1</v>
@@ -5155,15 +5155,15 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Gostaria de saber porque os créditos do cartão CME do meu filho nao foi creditado sendo que a mesma atende todos os critérios para o recebimento. Aluna: Maria Santos Fátima Vieira Ferreira, Data de nascimento: 12/12/2011 Nome da mãe: Betina Braga Souza CPF da mãe: 885.101.148-78 Nis:98765432165</t>
+          <t>Aconteceu um problema no meu computador e desde então não consigo encontrar e baixar o soft COMERCIOPLUS 2020. Estou com um enorme problema, pois durante todos esses anos os meus controles da minha propriedade comercial estão vinculados ao COMERCIOPLUS 2020. No momento estou sem acesso a todos os meus controles. Venho pedir encarecidamente a ajuda da DF Legal. Confiante na solução desse meu problema já agradeço atenção! OBS; Sou usuário do COMERCIOPLUS desde a versão 2012</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
@@ -5178,74 +5178,74 @@
         <v>0</v>
       </c>
       <c r="H97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J97" t="n">
         <v>1</v>
       </c>
       <c r="K97" t="n">
+        <v>0</v>
+      </c>
+      <c r="L97" t="n">
+        <v>1</v>
+      </c>
+      <c r="M97" t="n">
         <v>3</v>
       </c>
-      <c r="L97" t="n">
-        <v>0</v>
-      </c>
-      <c r="M97" t="n">
-        <v>1</v>
-      </c>
       <c r="N97" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Não consigo ter acesso ao Processo SEI 02510-25698413/2017-65 no Der que trata de reclamação sobre multa e apreensão indevida de carro. Não tenho acesso à conclusão do processo e decisão final do der.</t>
+          <t>Gostaria de saber porque os créditos do cartão CME do meu filho nao foi creditado sendo que a mesma atende todos os critérios para o recebimento. Aluna: Maria Santos Fátima Vieira Ferreira, Data de nascimento: 12/12/2011 Nome da mãe: Betina Braga Souza CPF da mãe: 885.101.148-78 Nis:98765432165</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K98" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L98" t="n">
         <v>0</v>
       </c>
       <c r="M98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N98" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O98" t="n">
         <v>1</v>
@@ -5253,50 +5253,99 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Não consigo ter acesso ao Processo SEI 02510-25698413/2017-65 no Der que trata de reclamação sobre multa e apreensão indevida de carro. Não tenho acesso à conclusão do processo e decisão final do der.</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>1</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
+      <c r="L99" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" t="n">
+        <v>0</v>
+      </c>
+      <c r="N99" t="n">
+        <v>2</v>
+      </c>
+      <c r="O99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
         <v>99</v>
       </c>
-      <c r="B99" t="inlineStr">
+      <c r="B100" t="inlineStr">
         <is>
           <t>Denúncia - e-Ouvidoria Canal de comunicação entre o cidadão e a administração pública. PROTOCOLO: 000254.2012-56 Informações do Pedido Razão Social: gestaojaira_ CNPJ: 48.236.147/0001-89 E-mail: feito10@press.so Secretaria: Contoladoria Geral Assunto: ASSÉDIO Data Pedido: 31/11/2012 Bairro Hortolândia Prazo de atendimento: 28/03/2024 Localização: Ministério Público do SP Descrição: CARTA PRECATÓRIA PARA TABOÃO DA SERRA. PARA QUE NÃO EXISTA ESBULHO OU ASSÉDIO MORAL: DENUNCIA LIGAÇÕES TELEFÔNICAS MUDAS. OCORRÊNCIA REGISTRADO NAS DELEGACIAS. COMUNICADO DO CIDADÃO CPF 551.169.500-18. Eduardo da Costa Barbosa (13/03/1956). Nascimento em Brasília, Distrito Federal. Número do telefone (95)99149-2006 e Whatsapp (97)99201-2009. Nome social (se for o caso); Nome da mãe e do pai; funcionária pública Pablo da Vitória Simões. Endereço residência à Avenida São Luís 333 Taboão da Serra SP CEP 29. 192 - 170. Condomínio Municipal Hélio Silva Campos * Motivo do pedido: Solicitação de providências após o registro de inúmeros e diversos boletins de ocorrências. VENDA DO IMÓVEL. Simplificando a denúncia para fiscalização e proteção municipal. Motivo do pedido MONITORAMENTO INCOMUM E REGISTROS DE NOVAS OCORRÊNCIAS. A liberdade de locomoção é um direito fundamental amplo, assegurado a qualquer ser humano, mas que tem suas limitações. Nossa Constituição trata do direito à liberdade de locomoção em vários momentos, conforme se verá. No art. 5º, XV da Constituição Federal está escrito o seguinte. MPSP:Protocolo realizado por Marcos Henrique da Silva Simoes, em nome de Edson Henrique da Costa Camargo. Os arquivos protocolados foram juntados nos autos Gampes nº 2012.01315.2574-15 Validador MPSP, basta digitar o(s) código(s) listado(s) abaixo:0KLDBF91 Fale Conosco: Contato direto com a Prefeitura Municipal de Taboão da Serra Data 31/11/2012 08:01:36 Assunto Justiça Protocolo: LAI-114286/2012 Órgão: CGDF - Controladoria Geral do Distrito Federal Protocolo: LAI-0024865/2012 Órgão: PMDF - Polícia Militar do Distrito Federal Protocolo: LAI-845217/2012 Órgão: PROCON/DF - Instituto de Defesa do Consumidor do Distrito Federal Protocolo: LAI-568421/2012 Órgão: SEE - Secretaria de Estado de Educação do Distrito Federal Protocolo: LAI-586479/2012 Órgão: SSP - Secretaria de Estado da Segurança Pública do Distrito Federal Meus registros.</t>
         </is>
       </c>
-      <c r="C99" t="n">
-        <v>1</v>
-      </c>
-      <c r="D99" t="n">
-        <v>1</v>
-      </c>
-      <c r="E99" t="n">
-        <v>1</v>
-      </c>
-      <c r="F99" t="n">
-        <v>1</v>
-      </c>
-      <c r="G99" t="n">
-        <v>1</v>
-      </c>
-      <c r="H99" t="n">
-        <v>1</v>
-      </c>
-      <c r="I99" t="n">
-        <v>1</v>
-      </c>
-      <c r="J99" t="n">
-        <v>1</v>
-      </c>
-      <c r="K99" t="n">
+      <c r="C100" t="n">
+        <v>1</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
+      <c r="E100" t="n">
+        <v>1</v>
+      </c>
+      <c r="F100" t="n">
+        <v>1</v>
+      </c>
+      <c r="G100" t="n">
+        <v>1</v>
+      </c>
+      <c r="H100" t="n">
+        <v>1</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1</v>
+      </c>
+      <c r="J100" t="n">
+        <v>1</v>
+      </c>
+      <c r="K100" t="n">
         <v>7</v>
       </c>
-      <c r="L99" t="n">
+      <c r="L100" t="n">
         <v>19</v>
       </c>
-      <c r="M99" t="n">
+      <c r="M100" t="n">
         <v>4</v>
       </c>
-      <c r="N99" t="n">
+      <c r="N100" t="n">
         <v>45</v>
       </c>
-      <c r="O99" t="n">
+      <c r="O100" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:sparkles: feat: Enhance CPF, CNPJ, and RG regex patterns and implement mathematical CPF validation for improved data integrity.
</commit_message>
<xml_diff>
--- a/data/processed/Hackathon Participa DF Data Processado.xlsx
+++ b/data/processed/Hackathon Participa DF Data Processado.xlsx
@@ -658,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -691,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -756,7 +756,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -765,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -789,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="O7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -814,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -949,10 +949,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -961,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
@@ -1108,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1687,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1696,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -1720,7 +1720,7 @@
         <v>2</v>
       </c>
       <c r="O26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1831,7 +1831,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1843,7 +1843,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
         <v>1</v>
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1965,7 +1965,7 @@
         <v>6</v>
       </c>
       <c r="O31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1981,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -2014,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -2030,7 +2030,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -2039,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2063,7 +2063,7 @@
         <v>5</v>
       </c>
       <c r="O33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2079,7 +2079,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="O34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -2128,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
         <v>1</v>
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -2333,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
         <v>0</v>
@@ -2357,7 +2357,7 @@
         <v>6</v>
       </c>
       <c r="O39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2373,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -2382,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -2406,7 +2406,7 @@
         <v>2</v>
       </c>
       <c r="O40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2422,7 +2422,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -2431,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -2455,7 +2455,7 @@
         <v>13</v>
       </c>
       <c r="O41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -2909,7 +2909,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
@@ -2921,7 +2921,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51" t="n">
         <v>1</v>
@@ -3117,7 +3117,7 @@
         <v>1</v>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55" t="n">
         <v>1</v>
@@ -3157,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -3166,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -3190,7 +3190,7 @@
         <v>1</v>
       </c>
       <c r="O56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -3264,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -3288,7 +3288,7 @@
         <v>7</v>
       </c>
       <c r="O58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -3350,7 +3350,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
         <v>0</v>
@@ -3402,7 +3402,7 @@
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
         <v>1</v>
@@ -3411,7 +3411,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -3448,7 +3448,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
@@ -3705,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -3729,7 +3729,7 @@
         <v>4</v>
       </c>
       <c r="O67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -3745,7 +3745,7 @@
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
@@ -3754,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -3778,7 +3778,7 @@
         <v>1</v>
       </c>
       <c r="O68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -3843,7 +3843,7 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
@@ -3852,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" t="n">
         <v>1</v>
@@ -3941,7 +3941,7 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
@@ -3950,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -3974,7 +3974,7 @@
         <v>1</v>
       </c>
       <c r="O72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -3990,7 +3990,7 @@
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
@@ -3999,7 +3999,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -4023,7 +4023,7 @@
         <v>4</v>
       </c>
       <c r="O73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -4036,10 +4036,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
@@ -4048,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" t="n">
         <v>1</v>
@@ -4186,7 +4186,7 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
@@ -4195,7 +4195,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77" t="n">
         <v>1</v>
@@ -4624,7 +4624,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
@@ -4636,7 +4636,7 @@
         <v>1</v>
       </c>
       <c r="G86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86" t="n">
         <v>1</v>
@@ -4676,7 +4676,7 @@
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
@@ -4685,7 +4685,7 @@
         <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -4709,7 +4709,7 @@
         <v>1</v>
       </c>
       <c r="O87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -4774,7 +4774,7 @@
         <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
@@ -4783,7 +4783,7 @@
         <v>0</v>
       </c>
       <c r="G89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89" t="n">
         <v>0</v>
@@ -4807,7 +4807,7 @@
         <v>8</v>
       </c>
       <c r="O89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -5028,7 +5028,7 @@
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94" t="n">
         <v>0</v>
@@ -5052,7 +5052,7 @@
         <v>21</v>
       </c>
       <c r="O94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -5117,7 +5117,7 @@
         <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" t="n">
         <v>1</v>
@@ -5126,7 +5126,7 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96" t="n">
         <v>0</v>
@@ -5212,7 +5212,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98" t="n">
         <v>0</v>
@@ -5264,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="D99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
@@ -5273,7 +5273,7 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -5297,7 +5297,7 @@
         <v>2</v>
       </c>
       <c r="O99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -5310,7 +5310,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" t="n">
         <v>1</v>
@@ -5322,7 +5322,7 @@
         <v>1</v>
       </c>
       <c r="G100" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
:wrench: fix: Refine Brazilian phone number regex to accurately validate fixed and mobile lines.
</commit_message>
<xml_diff>
--- a/data/processed/Hackathon Participa DF Data Processado.xlsx
+++ b/data/processed/Hackathon Participa DF Data Processado.xlsx
@@ -2967,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
@@ -2994,7 +2994,7 @@
         <v>1</v>
       </c>
       <c r="O52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -3506,7 +3506,7 @@
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
@@ -3533,7 +3533,7 @@
         <v>4</v>
       </c>
       <c r="O63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -4584,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G85" t="n">
         <v>0</v>
@@ -4611,7 +4611,7 @@
         <v>5</v>
       </c>
       <c r="O85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">

</xml_diff>

<commit_message>
Optimize NER processing with nlp.pipe and update processed data
</commit_message>
<xml_diff>
--- a/data/processed/Hackathon Participa DF Data Processado.xlsx
+++ b/data/processed/Hackathon Participa DF Data Processado.xlsx
@@ -682,13 +682,13 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
@@ -771,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -780,13 +780,13 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
@@ -823,19 +823,19 @@
         <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
         <v>2</v>
       </c>
       <c r="L8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O8" t="n">
         <v>1</v>
@@ -878,13 +878,13 @@
         <v>2</v>
       </c>
       <c r="L9" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O9" t="n">
         <v>1</v>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -927,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -970,19 +970,19 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O11" t="n">
         <v>1</v>
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
         <v>1</v>
@@ -1022,19 +1022,19 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N12" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -1074,13 +1074,13 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
@@ -1114,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
         <v>1</v>
@@ -1123,13 +1123,13 @@
         <v>2</v>
       </c>
       <c r="L14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O14" t="n">
         <v>1</v>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
         <v>1</v>
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
         <v>1</v>
@@ -1209,7 +1209,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
         <v>1</v>
@@ -1218,19 +1218,19 @@
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M16" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N16" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1261,19 +1261,19 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
         <v>1</v>
@@ -1316,16 +1316,16 @@
         <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L18" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M18" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N18" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="O18" t="n">
         <v>1</v>
@@ -1359,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1368,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" t="n">
         <v>0</v>
@@ -1411,16 +1411,16 @@
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" t="n">
         <v>3</v>
       </c>
       <c r="L20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N20" t="n">
         <v>10</v>
@@ -1466,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
@@ -1552,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
         <v>1</v>
@@ -1561,19 +1561,19 @@
         <v>1</v>
       </c>
       <c r="K23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M23" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N23" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="O23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1613,13 +1613,13 @@
         <v>2</v>
       </c>
       <c r="L24" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" t="n">
         <v>2</v>
       </c>
-      <c r="M24" t="n">
-        <v>3</v>
-      </c>
       <c r="N24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O24" t="n">
         <v>1</v>
@@ -1662,13 +1662,13 @@
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M25" t="n">
         <v>3</v>
       </c>
       <c r="N25" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="O25" t="n">
         <v>0</v>
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="N26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O26" t="n">
         <v>0</v>
@@ -1760,13 +1760,13 @@
         <v>1</v>
       </c>
       <c r="L27" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M27" t="n">
         <v>0</v>
       </c>
       <c r="N27" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O27" t="n">
         <v>1</v>
@@ -1800,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
         <v>1</v>
@@ -1809,13 +1809,13 @@
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" t="n">
+        <v>1</v>
+      </c>
+      <c r="N28" t="n">
         <v>2</v>
-      </c>
-      <c r="N28" t="n">
-        <v>6</v>
       </c>
       <c r="O28" t="n">
         <v>0</v>
@@ -1852,16 +1852,16 @@
         <v>1</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="n">
         <v>3</v>
       </c>
       <c r="L29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" t="n">
         <v>5</v>
@@ -1898,19 +1898,19 @@
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" t="n">
         <v>1</v>
@@ -1956,13 +1956,13 @@
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M31" t="n">
         <v>0</v>
       </c>
       <c r="N31" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O31" t="n">
         <v>0</v>
@@ -2011,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="N32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" t="n">
         <v>0</v>
@@ -2054,13 +2054,13 @@
         <v>0</v>
       </c>
       <c r="L33" t="n">
+        <v>2</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
         <v>4</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" t="n">
-        <v>5</v>
       </c>
       <c r="O33" t="n">
         <v>0</v>
@@ -2158,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O35" t="n">
         <v>1</v>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
         <v>1</v>
@@ -2201,13 +2201,13 @@
         <v>0</v>
       </c>
       <c r="L36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" t="n">
         <v>1</v>
       </c>
       <c r="N36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -2342,19 +2342,19 @@
         <v>1</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M39" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N39" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
@@ -2446,13 +2446,13 @@
         <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M41" t="n">
         <v>3</v>
       </c>
       <c r="N41" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="O41" t="n">
         <v>0</v>
@@ -2486,7 +2486,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
         <v>0</v>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
@@ -2535,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="n">
         <v>1</v>
@@ -2544,13 +2544,13 @@
         <v>0</v>
       </c>
       <c r="L43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43" t="n">
         <v>1</v>
       </c>
       <c r="N43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O43" t="n">
         <v>0</v>
@@ -2593,13 +2593,13 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M44" t="n">
         <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O44" t="n">
         <v>0</v>
@@ -2645,10 +2645,10 @@
         <v>0</v>
       </c>
       <c r="M45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O45" t="n">
         <v>1</v>
@@ -2682,19 +2682,19 @@
         <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" t="n">
         <v>0</v>
       </c>
       <c r="L46" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M46" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N46" t="n">
         <v>5</v>
@@ -2746,7 +2746,7 @@
         <v>6</v>
       </c>
       <c r="N47" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O47" t="n">
         <v>0</v>
@@ -2789,13 +2789,13 @@
         <v>3</v>
       </c>
       <c r="L48" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M48" t="n">
         <v>1</v>
       </c>
       <c r="N48" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O48" t="n">
         <v>1</v>
@@ -2936,10 +2936,10 @@
         <v>1</v>
       </c>
       <c r="L51" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N51" t="n">
         <v>10</v>
@@ -2976,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="n">
         <v>0</v>
@@ -2985,7 +2985,7 @@
         <v>0</v>
       </c>
       <c r="L52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M52" t="n">
         <v>0</v>
@@ -3034,13 +3034,13 @@
         <v>2</v>
       </c>
       <c r="L53" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M53" t="n">
         <v>1</v>
       </c>
       <c r="N53" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="O53" t="n">
         <v>1</v>
@@ -3089,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="N54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O54" t="n">
         <v>0</v>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="H55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
@@ -3129,16 +3129,16 @@
         <v>1</v>
       </c>
       <c r="K55" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L55" t="n">
         <v>0</v>
       </c>
       <c r="M55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N55" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="O55" t="n">
         <v>1</v>
@@ -3230,13 +3230,13 @@
         <v>0</v>
       </c>
       <c r="L57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M57" t="n">
         <v>2</v>
       </c>
       <c r="N57" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O57" t="n">
         <v>0</v>
@@ -3279,13 +3279,13 @@
         <v>0</v>
       </c>
       <c r="L58" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M58" t="n">
         <v>2</v>
       </c>
       <c r="N58" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O58" t="n">
         <v>0</v>
@@ -3322,16 +3322,16 @@
         <v>1</v>
       </c>
       <c r="J59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K59" t="n">
         <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N59" t="n">
         <v>3</v>
@@ -3371,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K60" t="n">
         <v>1</v>
@@ -3380,7 +3380,7 @@
         <v>1</v>
       </c>
       <c r="M60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N60" t="n">
         <v>4</v>
@@ -3481,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="N62" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O62" t="n">
         <v>1</v>
@@ -3515,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" t="n">
         <v>0</v>
@@ -3524,13 +3524,13 @@
         <v>0</v>
       </c>
       <c r="L63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M63" t="n">
         <v>0</v>
       </c>
       <c r="N63" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O63" t="n">
         <v>0</v>
@@ -3561,19 +3561,19 @@
         <v>0</v>
       </c>
       <c r="H64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" t="n">
         <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M64" t="n">
         <v>0</v>
@@ -3582,7 +3582,7 @@
         <v>1</v>
       </c>
       <c r="O64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -3616,7 +3616,7 @@
         <v>1</v>
       </c>
       <c r="J65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K65" t="n">
         <v>0</v>
@@ -3625,7 +3625,7 @@
         <v>1</v>
       </c>
       <c r="M65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N65" t="n">
         <v>3</v>
@@ -3677,7 +3677,7 @@
         <v>0</v>
       </c>
       <c r="N66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O66" t="n">
         <v>1</v>
@@ -3720,13 +3720,13 @@
         <v>0</v>
       </c>
       <c r="L67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M67" t="n">
         <v>0</v>
       </c>
       <c r="N67" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O67" t="n">
         <v>0</v>
@@ -3763,7 +3763,7 @@
         <v>0</v>
       </c>
       <c r="J68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K68" t="n">
         <v>0</v>
@@ -3772,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="M68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N68" t="n">
         <v>1</v>
@@ -3858,7 +3858,7 @@
         <v>1</v>
       </c>
       <c r="I70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J70" t="n">
         <v>1</v>
@@ -3867,13 +3867,13 @@
         <v>1</v>
       </c>
       <c r="L70" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="n">
         <v>2</v>
       </c>
-      <c r="M70" t="n">
-        <v>1</v>
-      </c>
       <c r="N70" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O70" t="n">
         <v>1</v>
@@ -3922,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="N71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O71" t="n">
         <v>0</v>
@@ -3956,7 +3956,7 @@
         <v>0</v>
       </c>
       <c r="I72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72" t="n">
         <v>0</v>
@@ -3965,13 +3965,13 @@
         <v>0</v>
       </c>
       <c r="L72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M72" t="n">
         <v>0</v>
       </c>
       <c r="N72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O72" t="n">
         <v>0</v>
@@ -4017,10 +4017,10 @@
         <v>1</v>
       </c>
       <c r="M73" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N73" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O73" t="n">
         <v>0</v>
@@ -4060,16 +4060,16 @@
         <v>1</v>
       </c>
       <c r="K74" t="n">
+        <v>1</v>
+      </c>
+      <c r="L74" t="n">
+        <v>1</v>
+      </c>
+      <c r="M74" t="n">
         <v>2</v>
       </c>
-      <c r="L74" t="n">
-        <v>2</v>
-      </c>
-      <c r="M74" t="n">
-        <v>1</v>
-      </c>
       <c r="N74" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O74" t="n">
         <v>1</v>
@@ -4103,7 +4103,7 @@
         <v>0</v>
       </c>
       <c r="I75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J75" t="n">
         <v>0</v>
@@ -4112,13 +4112,13 @@
         <v>0</v>
       </c>
       <c r="L75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M75" t="n">
         <v>0</v>
       </c>
       <c r="N75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O75" t="n">
         <v>0</v>
@@ -4161,13 +4161,13 @@
         <v>0</v>
       </c>
       <c r="L76" t="n">
+        <v>1</v>
+      </c>
+      <c r="M76" t="n">
+        <v>1</v>
+      </c>
+      <c r="N76" t="n">
         <v>4</v>
-      </c>
-      <c r="M76" t="n">
-        <v>1</v>
-      </c>
-      <c r="N76" t="n">
-        <v>7</v>
       </c>
       <c r="O76" t="n">
         <v>0</v>
@@ -4207,16 +4207,16 @@
         <v>1</v>
       </c>
       <c r="K77" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L77" t="n">
         <v>1</v>
       </c>
       <c r="M77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N77" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="O77" t="n">
         <v>1</v>
@@ -4253,7 +4253,7 @@
         <v>1</v>
       </c>
       <c r="J78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K78" t="n">
         <v>0</v>
@@ -4262,10 +4262,10 @@
         <v>1</v>
       </c>
       <c r="M78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O78" t="n">
         <v>0</v>
@@ -4296,7 +4296,7 @@
         <v>0</v>
       </c>
       <c r="H79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I79" t="n">
         <v>1</v>
@@ -4305,19 +4305,19 @@
         <v>0</v>
       </c>
       <c r="K79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L79" t="n">
+        <v>2</v>
+      </c>
+      <c r="M79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" t="n">
         <v>3</v>
       </c>
-      <c r="M79" t="n">
-        <v>0</v>
-      </c>
-      <c r="N79" t="n">
-        <v>4</v>
-      </c>
       <c r="O79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -4455,13 +4455,13 @@
         <v>0</v>
       </c>
       <c r="L82" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M82" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N82" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="O82" t="n">
         <v>0</v>
@@ -4498,19 +4498,19 @@
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K83" t="n">
         <v>0</v>
       </c>
       <c r="L83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N83" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O83" t="n">
         <v>0</v>
@@ -4541,7 +4541,7 @@
         <v>0</v>
       </c>
       <c r="H84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="n">
         <v>1</v>
@@ -4550,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="K84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L84" t="n">
         <v>1</v>
@@ -4559,10 +4559,10 @@
         <v>0</v>
       </c>
       <c r="N84" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -4596,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="J85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K85" t="n">
         <v>0</v>
@@ -4605,10 +4605,10 @@
         <v>1</v>
       </c>
       <c r="M85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N85" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O85" t="n">
         <v>0</v>
@@ -4645,19 +4645,19 @@
         <v>1</v>
       </c>
       <c r="J86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L86" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N86" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O86" t="n">
         <v>1</v>
@@ -4706,7 +4706,7 @@
         <v>0</v>
       </c>
       <c r="N87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O87" t="n">
         <v>0</v>
@@ -4743,19 +4743,19 @@
         <v>1</v>
       </c>
       <c r="J88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L88" t="n">
         <v>2</v>
       </c>
       <c r="M88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N88" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O88" t="n">
         <v>1</v>
@@ -4798,13 +4798,13 @@
         <v>0</v>
       </c>
       <c r="L89" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N89" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O89" t="n">
         <v>0</v>
@@ -4853,7 +4853,7 @@
         <v>0</v>
       </c>
       <c r="N90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O90" t="n">
         <v>0</v>
@@ -4890,7 +4890,7 @@
         <v>1</v>
       </c>
       <c r="J91" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K91" t="n">
         <v>8</v>
@@ -4899,10 +4899,10 @@
         <v>5</v>
       </c>
       <c r="M91" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N91" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O91" t="n">
         <v>1</v>
@@ -4982,7 +4982,7 @@
         <v>0</v>
       </c>
       <c r="H93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" t="n">
         <v>1</v>
@@ -4991,19 +4991,19 @@
         <v>1</v>
       </c>
       <c r="K93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L93" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M93" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N93" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="O93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -5043,13 +5043,13 @@
         <v>0</v>
       </c>
       <c r="L94" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M94" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N94" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O94" t="n">
         <v>0</v>
@@ -5083,22 +5083,22 @@
         <v>0</v>
       </c>
       <c r="I95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K95" t="n">
         <v>0</v>
       </c>
       <c r="L95" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M95" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N95" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O95" t="n">
         <v>0</v>
@@ -5135,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K96" t="n">
         <v>0</v>
@@ -5144,10 +5144,10 @@
         <v>0</v>
       </c>
       <c r="M96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N96" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O96" t="n">
         <v>1</v>
@@ -5184,7 +5184,7 @@
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K97" t="n">
         <v>0</v>
@@ -5193,10 +5193,10 @@
         <v>1</v>
       </c>
       <c r="M97" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N97" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O97" t="n">
         <v>0</v>
@@ -5245,7 +5245,7 @@
         <v>1</v>
       </c>
       <c r="N98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O98" t="n">
         <v>1</v>
@@ -5279,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="I99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J99" t="n">
         <v>0</v>
@@ -5288,7 +5288,7 @@
         <v>0</v>
       </c>
       <c r="L99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M99" t="n">
         <v>0</v>
@@ -5334,16 +5334,16 @@
         <v>1</v>
       </c>
       <c r="K100" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L100" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="M100" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N100" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="O100" t="n">
         <v>1</v>

</xml_diff>